<commit_message>
Update on 20200106 evening
</commit_message>
<xml_diff>
--- a/文档/其他文档/Others/Games/Levels and stars on King of Glory.xlsx
+++ b/文档/其他文档/Others/Games/Levels and stars on King of Glory.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -279,12 +279,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -326,7 +329,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -361,7 +364,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -576,15 +579,15 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="36.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -911,7 +914,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -924,7 +927,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>